<commit_message>
Commit REQ9332_TST960, it need to be perfect after the AddDevice method is modified.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST2755_IntervalForGlobalStatusPolling.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST2755_IntervalForGlobalStatusPolling.xlsx
@@ -1278,7 +1278,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7925" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7925" uniqueCount="893">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4003,6 +4003,10 @@
   </si>
   <si>
     <t>$GXT_Ip_Port$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{CONTROL down}{Akey}{CONTROL up}"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4234,21 +4238,7 @@
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -4555,8 +4545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="B76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6428,7 +6418,7 @@
         <v>3</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>838</v>
+        <v>892</v>
       </c>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
@@ -6512,10 +6502,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N1:N79">
-    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>